<commit_message>
Corrections to metadata files. Litter structural C used DecayRateSurf as maximum. Variable BiomassToLAI changed to LeafBiomassToLAI. Documentation updated.
</commit_message>
<xml_diff>
--- a/docs/NECN_Functional_Table.xlsx
+++ b/docs/NECN_Functional_Table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rschell\Google Drive\Teaching\NECN Training 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rschell\Documents\LANDIS-Git\Extension-NECN-Succession\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13515"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13512"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>FractionANPPtoLeaf</t>
   </si>
   <si>
-    <t>BiomassToLAI</t>
-  </si>
-  <si>
     <t>KLAI</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Biogeochemical Attributes</t>
+  </si>
+  <si>
+    <t>LeafBiomassToLAI</t>
   </si>
 </sst>
 </file>
@@ -535,20 +535,20 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="19" width="12.7109375" customWidth="1"/>
+    <col min="1" max="19" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -563,45 +563,45 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -655,9 +655,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -711,9 +711,9 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -767,39 +767,39 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="8" t="s">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C11" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="D11" s="4"/>
     </row>

</xml_diff>